<commit_message>
changed : on dataset variables, dont show columns dataset, folder and institution
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>2011</t>
+  </si>
+  <si>
+    <t>dep_sante___variable_3</t>
   </si>
 </sst>
 </file>
@@ -394,6 +397,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>1746359037</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added : value link color on hover
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t>dep_sante___variable_3</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_1</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_25</t>
+  </si>
+  <si>
+    <t>accident_route___variable_4</t>
   </si>
 </sst>
 </file>
@@ -420,6 +435,66 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10">
+        <v>1746734601</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1746734601</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>1746734601</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added : institution valididy start and end date
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -179,6 +179,30 @@
   </si>
   <si>
     <t>vide</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>dfi</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>dff</t>
+  </si>
+  <si>
+    <t>2010/10</t>
+  </si>
+  <si>
+    <t>seco</t>
+  </si>
+  <si>
+    <t>2021/04</t>
   </si>
 </sst>
 </file>
@@ -704,6 +728,86 @@
         <v>12</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23">
+        <v>1747340787</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>1747340787</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>1747340787</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>1747340787</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add : data lineage at the variable level and infered for the dataset level
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -203,6 +203,57 @@
   </si>
   <si>
     <t>2021/04</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_12</t>
+  </si>
+  <si>
+    <t>source_var_ids</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_10, ser_pub_loc___variable_11</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>config</t>
+  </si>
+  <si>
+    <t>alias_3</t>
+  </si>
+  <si>
+    <t>sourceVar_ids</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>variable : source_var</t>
+  </si>
+  <si>
+    <t>variable : sourceVar</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>source_ids</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_14</t>
+  </si>
+  <si>
+    <t>accident_route___variable_7, dep_sante___variable_7</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_15</t>
+  </si>
+  <si>
+    <t>accident_route___variable_7</t>
   </si>
 </sst>
 </file>
@@ -808,6 +859,333 @@
         <v>63</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27">
+        <v>1747906147</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>1747906281</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>1747906551</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>1747906551</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>1747906566</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>1747907576</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>1747907576</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>1747907625</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>1747907625</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>1747913177</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>1747913221</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>1747913221</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>1747913314</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
+        <v>75</v>
+      </c>
+      <c r="G39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>1747913314</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+      <c r="H40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>1747918633</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="H41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>1747921769</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1747921769</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" t="s">
+        <v>70</v>
+      </c>
+      <c r="H43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>1747921769</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" t="s">
+        <v>70</v>
+      </c>
+      <c r="H44" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add : switch show tree on tag item page
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>accident_route___variable_7</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>images_aeriennes_1</t>
+  </si>
+  <si>
+    <t>images_aeriennes_2</t>
   </si>
 </sst>
 </file>
@@ -1186,6 +1195,34 @@
         <v>80</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45">
+        <v>1749897806</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>1749897806</v>
+      </c>
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add : freq tab and column for variables with visual frequency distribution
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -263,6 +263,111 @@
   </si>
   <si>
     <t>images_aeriennes_2</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>variable_1---null</t>
+  </si>
+  <si>
+    <t>variable_1---value_1</t>
+  </si>
+  <si>
+    <t>variable_1---value_2</t>
+  </si>
+  <si>
+    <t>accident_route___variable_1---value</t>
+  </si>
+  <si>
+    <t>accident_route___variable_1---value_1</t>
+  </si>
+  <si>
+    <t>accident_route___variable_1---value_2</t>
+  </si>
+  <si>
+    <t>accident_route___variable_1---value_3</t>
+  </si>
+  <si>
+    <t>variable_1</t>
+  </si>
+  <si>
+    <t>accident_route___variable_13---value</t>
+  </si>
+  <si>
+    <t>accident_route___variable_13---value_1</t>
+  </si>
+  <si>
+    <t>accident_route___variable_13---value_2</t>
+  </si>
+  <si>
+    <t>accident_route___variable_13---value_3</t>
+  </si>
+  <si>
+    <t>accident_route___variable_1</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_1</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_2</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_3</t>
+  </si>
+  <si>
+    <t>accident_route___variable_13</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_4</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_5</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_6</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_7</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_8</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_9</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_10</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_11</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_12</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_13</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_14</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_2 long with a lot of text</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_2 long with a lot of text, but like a lot of text very very very</t>
+  </si>
+  <si>
+    <t>ser_pub_loc___variable_13---value_2 long with a lot of text, but like a lot of text very very very value_2 long with a lot of text, but like a lot of text very very very</t>
   </si>
 </sst>
 </file>
@@ -1223,6 +1328,704 @@
         <v>83</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47">
+        <v>1753871814</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>1753871814</v>
+      </c>
+      <c r="B48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>1753871814</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>1753871964</v>
+      </c>
+      <c r="B50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>1753871964</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>1753871964</v>
+      </c>
+      <c r="B52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>1753871964</v>
+      </c>
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>1753871964</v>
+      </c>
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" t="s">
+        <v>85</v>
+      </c>
+      <c r="E54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>1753871964</v>
+      </c>
+      <c r="B55" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>1753871964</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>1753874536</v>
+      </c>
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>1753874536</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>1753874536</v>
+      </c>
+      <c r="B59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>1753874536</v>
+      </c>
+      <c r="B60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>1753874536</v>
+      </c>
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>1753874536</v>
+      </c>
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>1753874536</v>
+      </c>
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>1753874536</v>
+      </c>
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>1753874564</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>1753874564</v>
+      </c>
+      <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>1753874564</v>
+      </c>
+      <c r="B67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>1753874564</v>
+      </c>
+      <c r="B68" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>1753874564</v>
+      </c>
+      <c r="B69" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" t="s">
+        <v>93</v>
+      </c>
+      <c r="E69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>1753874564</v>
+      </c>
+      <c r="B70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" t="s">
+        <v>94</v>
+      </c>
+      <c r="E70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>1753874564</v>
+      </c>
+      <c r="B71" t="s">
+        <v>43</v>
+      </c>
+      <c r="C71" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" t="s">
+        <v>95</v>
+      </c>
+      <c r="E71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>1753874564</v>
+      </c>
+      <c r="B72" t="s">
+        <v>43</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" t="s">
+        <v>96</v>
+      </c>
+      <c r="E72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>1753875837</v>
+      </c>
+      <c r="B73" t="s">
+        <v>67</v>
+      </c>
+      <c r="C73" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>1753875837</v>
+      </c>
+      <c r="B74" t="s">
+        <v>67</v>
+      </c>
+      <c r="C74" t="s">
+        <v>84</v>
+      </c>
+      <c r="D74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>1753875837</v>
+      </c>
+      <c r="B75" t="s">
+        <v>67</v>
+      </c>
+      <c r="C75" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>1753875837</v>
+      </c>
+      <c r="B76" t="s">
+        <v>67</v>
+      </c>
+      <c r="C76" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>1753875837</v>
+      </c>
+      <c r="B77" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>1753875837</v>
+      </c>
+      <c r="B78" t="s">
+        <v>67</v>
+      </c>
+      <c r="C78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>1753875837</v>
+      </c>
+      <c r="B79" t="s">
+        <v>67</v>
+      </c>
+      <c r="C79" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>1753875837</v>
+      </c>
+      <c r="B80" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>1753875837</v>
+      </c>
+      <c r="B81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C81" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>1753875837</v>
+      </c>
+      <c r="B82" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>1753875837</v>
+      </c>
+      <c r="B83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>1753875837</v>
+      </c>
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>84</v>
+      </c>
+      <c r="D84" t="s">
+        <v>98</v>
+      </c>
+      <c r="F84" t="s">
+        <v>84</v>
+      </c>
+      <c r="G84" t="s">
+        <v>114</v>
+      </c>
+      <c r="H84" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>1753876042</v>
+      </c>
+      <c r="B85" t="s">
+        <v>67</v>
+      </c>
+      <c r="C85" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>1753876042</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" t="s">
+        <v>100</v>
+      </c>
+      <c r="E86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>1753876086</v>
+      </c>
+      <c r="B87" t="s">
+        <v>67</v>
+      </c>
+      <c r="C87" t="s">
+        <v>84</v>
+      </c>
+      <c r="D87" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>1753876086</v>
+      </c>
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>84</v>
+      </c>
+      <c r="D88" t="s">
+        <v>116</v>
+      </c>
+      <c r="E88" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>1753876146</v>
+      </c>
+      <c r="B89" t="s">
+        <v>67</v>
+      </c>
+      <c r="C89" t="s">
+        <v>84</v>
+      </c>
+      <c r="D89" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>1753876146</v>
+      </c>
+      <c r="B90" t="s">
+        <v>43</v>
+      </c>
+      <c r="C90" t="s">
+        <v>84</v>
+      </c>
+      <c r="D90" t="s">
+        <v>117</v>
+      </c>
+      <c r="E90" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>1753879819</v>
+      </c>
+      <c r="B91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" t="s">
+        <v>84</v>
+      </c>
+      <c r="D91" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>1753879819</v>
+      </c>
+      <c r="B92" t="s">
+        <v>43</v>
+      </c>
+      <c r="C92" t="s">
+        <v>84</v>
+      </c>
+      <c r="D92" t="s">
+        <v>118</v>
+      </c>
+      <c r="E92" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change : jsonjs db data default to non compact mode
</commit_message>
<xml_diff>
--- a/public/data/db_source/evolution.xlsx
+++ b/public/data/db_source/evolution.xlsx
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>ser_pub_loc___variable_13---value_2 long with a lot of text, but like a lot of text very very very value_2 long with a lot of text, but like a lot of text very very very</t>
+  </si>
+  <si>
+    <t>2021/05</t>
   </si>
 </sst>
 </file>
@@ -2026,6 +2029,29 @@
         <v>76</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93">
+        <v>1757018090</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" t="s">
+        <v>56</v>
+      </c>
+      <c r="D93" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" t="s">
+        <v>63</v>
+      </c>
+      <c r="H93" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>